<commit_message>
Added HR.idf and modified run_energyplus_single as ExpandObjects.txt not required for HR.idf. Modified replace.xlsx for HR. Added main for testing.
</commit_message>
<xml_diff>
--- a/data/replace.xlsx
+++ b/data/replace.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrenis\gitprojects\BuildME\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7159A953-A120-4FEF-8DC4-869BACF7822F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58098CD1-DA59-4B9D-B99D-4CA9FD5C475B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{F14F42AE-B2B5-F34E-80E7-10F24B944563}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="25050" windowHeight="12915" activeTab="1" xr2:uid="{F14F42AE-B2B5-F34E-80E7-10F24B944563}"/>
   </bookViews>
   <sheets>
     <sheet name="RES" sheetId="3" r:id="rId1"/>
@@ -987,7 +987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA82845-CEEF-7E4F-96E4-0B03017A75CF}">
   <dimension ref="A1:H323"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>